<commit_message>
finished excel populate script
</commit_message>
<xml_diff>
--- a/Blank Time Sheet.xlsx
+++ b/Blank Time Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Projects\email-Excel-Timesheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Projects\autoTimeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E228EC-C5B3-43F7-8BD7-9D15148125B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CAEF0E-1FC9-4305-9574-3A3AAC175E45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Front" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t xml:space="preserve">Stark, Chad </t>
-  </si>
-  <si>
     <t>Pay period Start:</t>
   </si>
   <si>
@@ -177,22 +174,55 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>1/16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/3/2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/16/2021</t>
+    <t xml:space="preserve">1/4/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/17/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/17</t>
   </si>
   <si>
     <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1/31</t>
   </si>
 </sst>
 </file>
@@ -1244,6 +1274,62 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1265,69 +1351,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="37" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1690,193 +1720,213 @@
   <sheetPr/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="140" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="15" width="4.7109375" style="1" customWidth="1"/>
-    <col min="16" max="16" width="3.28515625" style="4" customWidth="1"/>
+    <col min="2" max="15" width="4.6640625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="3.33203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s" s="111">
+    <row r="1" spans="1:21" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="99"/>
+      <c r="G2" t="s" s="96">
         <v>0</v>
       </c>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
-      <c r="F2" s="113"/>
-      <c r="G2" t="s" s="110">
+      <c r="H2" s="92"/>
+      <c r="I2" t="s" s="93">
+        <v>47</v>
+      </c>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
+      <c r="L2" s="95"/>
+      <c r="M2" t="s" s="91">
         <v>1</v>
       </c>
-      <c r="H2" s="106"/>
-      <c r="I2" t="s" s="107">
-        <v>49</v>
-      </c>
-      <c r="J2" s="108"/>
-      <c r="K2" s="108"/>
-      <c r="L2" s="109"/>
-      <c r="M2" t="s" s="105">
+      <c r="N2" s="92"/>
+      <c r="O2" t="s" s="103">
+        <v>48</v>
+      </c>
+      <c r="P2" s="94"/>
+      <c r="Q2" s="104"/>
+    </row>
+    <row r="3" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s" s="51">
         <v>2</v>
       </c>
-      <c r="N2" s="106"/>
-      <c r="O2" t="s" s="116">
-        <v>50</v>
-      </c>
-      <c r="P2" s="108"/>
-      <c r="Q2" s="117"/>
-    </row>
-    <row r="3" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s" s="51">
+      <c r="B3" t="s" s="30">
         <v>3</v>
       </c>
-      <c r="B3" t="s" s="30">
+      <c r="C3" t="s" s="14">
         <v>4</v>
       </c>
-      <c r="C3" t="s" s="14">
+      <c r="D3" t="s" s="14">
         <v>5</v>
       </c>
-      <c r="D3" t="s" s="14">
+      <c r="E3" t="s" s="54">
         <v>6</v>
       </c>
-      <c r="E3" t="s" s="54">
+      <c r="F3" t="s" s="14">
         <v>7</v>
       </c>
-      <c r="F3" t="s" s="14">
+      <c r="G3" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="G3" t="s" s="14">
+      <c r="H3" t="s" s="14">
         <v>9</v>
       </c>
-      <c r="H3" t="s" s="14">
-        <v>10</v>
-      </c>
       <c r="I3" t="s" s="14">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s" s="78">
         <v>4</v>
       </c>
-      <c r="J3" t="s" s="78">
+      <c r="K3" t="s" s="14">
         <v>5</v>
       </c>
-      <c r="K3" t="s" s="14">
+      <c r="L3" t="s" s="14">
         <v>6</v>
       </c>
-      <c r="L3" t="s" s="14">
+      <c r="M3" t="s" s="14">
         <v>7</v>
       </c>
-      <c r="M3" t="s" s="14">
+      <c r="N3" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="N3" t="s" s="14">
+      <c r="O3" t="s" s="14">
         <v>9</v>
-      </c>
-      <c r="O3" t="s" s="14">
-        <v>10</v>
       </c>
       <c r="P3" s="12"/>
       <c r="Q3" t="s" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s" s="37">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="37">
-        <v>12</v>
-      </c>
       <c r="B4" t="s" s="39">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s" s="22">
+        <v>50</v>
+      </c>
+      <c r="D4" t="s" s="3">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s" s="3">
         <v>52</v>
       </c>
-      <c r="C4" t="s" s="22">
+      <c r="F4" t="s" s="3">
         <v>53</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
+      <c r="G4" t="s" s="3">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s" s="28">
+        <v>55</v>
+      </c>
+      <c r="I4" t="s" s="22">
+        <v>56</v>
+      </c>
+      <c r="J4" t="s" s="3">
+        <v>57</v>
+      </c>
+      <c r="K4" t="s" s="3">
+        <v>58</v>
+      </c>
+      <c r="L4" t="s" s="3">
+        <v>59</v>
+      </c>
+      <c r="M4" t="s" s="3">
+        <v>60</v>
+      </c>
+      <c r="N4" t="s" s="3">
+        <v>61</v>
+      </c>
       <c r="O4" t="s" s="3">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="P4" s="5"/>
       <c r="Q4" s="6"/>
     </row>
-    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s" s="48">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s" s="105">
         <v>13</v>
       </c>
-      <c r="B5" t="s" s="99">
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
+      <c r="E5" s="106"/>
+      <c r="F5" s="106"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="107"/>
+      <c r="Q5" s="85"/>
+    </row>
+    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s" s="41">
         <v>14</v>
       </c>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="85"/>
-    </row>
-    <row r="6" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s" s="41">
-        <v>15</v>
-      </c>
       <c r="B6" t="s" s="57">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s" s="57">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D6" s="73"/>
       <c r="E6" s="73"/>
       <c r="F6" t="s" s="57">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s" s="57">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="H6" t="s" s="57">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="I6" t="s" s="80">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="J6" t="s" s="57">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="K6" s="73"/>
       <c r="L6" s="73"/>
       <c r="M6" t="s" s="57">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="N6" t="s" s="57">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="O6" t="s" s="57">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="P6" s="12"/>
       <c r="Q6" s="79">
         <f>SUM(B6,C6,D6,E6,F6,G6,H6,I6,J6,K6,L6,M6,N6,O6)</f>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s" s="61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="39"/>
       <c r="C7" s="22"/>
@@ -1898,9 +1948,9 @@
       </c>
       <c r="S7" s="4"/>
     </row>
-    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s" s="56">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="40"/>
       <c r="C8" s="27"/>
@@ -1921,33 +1971,33 @@
         <f>SUM(B8,C8,D8,E8,F8,G8,H8,I8,J8,K8,L8,M8,N8,O8)</f>
       </c>
     </row>
-    <row r="9" spans="1:21" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" s="2" customFormat="1" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s" s="48">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s" s="100">
         <v>18</v>
       </c>
-      <c r="B9" t="s" s="95">
-        <v>19</v>
-      </c>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
-      <c r="J9" s="114"/>
-      <c r="K9" s="114"/>
-      <c r="L9" s="114"/>
-      <c r="M9" s="114"/>
-      <c r="N9" s="114"/>
-      <c r="O9" s="115"/>
+      <c r="C9" s="101"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="101"/>
+      <c r="M9" s="101"/>
+      <c r="N9" s="101"/>
+      <c r="O9" s="102"/>
       <c r="P9" s="47"/>
       <c r="Q9" s="24"/>
       <c r="T9" s="25"/>
     </row>
-    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s" s="43">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="58"/>
       <c r="C10" s="33"/>
@@ -1968,32 +2018,32 @@
         <f>SUM(B10,C10,D10,E10,F10,G10,H10,I10,J10,K10,L10,M10,N10,O10)</f>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s" s="71">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s" s="88">
         <v>20</v>
       </c>
-      <c r="B11" t="s" s="102">
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
+      <c r="I11" s="89"/>
+      <c r="J11" s="89"/>
+      <c r="K11" s="89"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
+      <c r="N11" s="89"/>
+      <c r="O11" s="89"/>
+      <c r="P11" s="90"/>
+      <c r="Q11" s="72"/>
+    </row>
+    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s" s="41">
         <v>21</v>
-      </c>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="103"/>
-      <c r="G11" s="103"/>
-      <c r="H11" s="103"/>
-      <c r="I11" s="103"/>
-      <c r="J11" s="103"/>
-      <c r="K11" s="103"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="103"/>
-      <c r="N11" s="103"/>
-      <c r="O11" s="103"/>
-      <c r="P11" s="104"/>
-      <c r="Q11" s="72"/>
-    </row>
-    <row r="12" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s" s="41">
-        <v>22</v>
       </c>
       <c r="B12" s="42"/>
       <c r="C12" s="30"/>
@@ -2014,9 +2064,9 @@
         <f>SUM(B12,C12,D12,E12,F12,G12,H12,I12,J12,K12,L12,M12,N12,O12)</f>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s" s="37">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="39"/>
       <c r="C13" s="22"/>
@@ -2037,9 +2087,9 @@
         <f>SUM(B13,C13,D13,E13,F13,G13,H13,I13,J13,K13,L13,M13,N13,O13)</f>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s" s="38">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="46"/>
       <c r="C14" s="27"/>
@@ -2060,9 +2110,9 @@
         <f>SUM(B14,C14,D14,E14,F14,G14,H14,I14,J14,K14,L14,M14,N14,O14)</f>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s" s="38">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="46"/>
       <c r="C15" s="27"/>
@@ -2084,9 +2134,9 @@
       </c>
       <c r="U15" s="4"/>
     </row>
-    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s" s="56">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="40"/>
       <c r="C16" s="27"/>
@@ -2107,53 +2157,53 @@
         <f>SUM(B16,C16,D16,E16,F16,G16,H16,I16,J16,K16,L16,M16,N16,O16)</f>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s" s="92">
+    <row r="17" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s" s="112">
+        <v>26</v>
+      </c>
+      <c r="B17" s="113"/>
+      <c r="C17" s="113"/>
+      <c r="D17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="113"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="113"/>
+      <c r="J17" s="113"/>
+      <c r="K17" s="113"/>
+      <c r="L17" s="113"/>
+      <c r="M17" s="113"/>
+      <c r="N17" s="113"/>
+      <c r="O17" s="113"/>
+      <c r="P17" s="113"/>
+      <c r="Q17" s="114"/>
+    </row>
+    <row r="18" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s" s="50">
         <v>27</v>
       </c>
-      <c r="B17" s="93"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="93"/>
-      <c r="E17" s="93"/>
-      <c r="F17" s="93"/>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
-      <c r="I17" s="93"/>
-      <c r="J17" s="93"/>
-      <c r="K17" s="93"/>
-      <c r="L17" s="93"/>
-      <c r="M17" s="93"/>
-      <c r="N17" s="93"/>
-      <c r="O17" s="93"/>
-      <c r="P17" s="93"/>
-      <c r="Q17" s="94"/>
-    </row>
-    <row r="18" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s" s="50">
+      <c r="B18" t="s" s="100">
         <v>28</v>
       </c>
-      <c r="B18" t="s" s="95">
-        <v>29</v>
-      </c>
-      <c r="C18" s="96"/>
-      <c r="D18" s="96"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="96"/>
-      <c r="G18" s="96"/>
-      <c r="H18" s="96"/>
-      <c r="I18" s="96"/>
-      <c r="J18" s="96"/>
-      <c r="K18" s="96"/>
-      <c r="L18" s="96"/>
-      <c r="M18" s="96"/>
-      <c r="N18" s="96"/>
-      <c r="O18" s="96"/>
-      <c r="P18" s="97"/>
+      <c r="C18" s="106"/>
+      <c r="D18" s="106"/>
+      <c r="E18" s="106"/>
+      <c r="F18" s="106"/>
+      <c r="G18" s="106"/>
+      <c r="H18" s="106"/>
+      <c r="I18" s="106"/>
+      <c r="J18" s="106"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="106"/>
+      <c r="M18" s="106"/>
+      <c r="N18" s="106"/>
+      <c r="O18" s="106"/>
+      <c r="P18" s="107"/>
       <c r="Q18" s="23"/>
     </row>
-    <row r="19" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s" s="41">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="42"/>
       <c r="C19" s="30"/>
@@ -2172,9 +2222,9 @@
       <c r="P19" s="12"/>
       <c r="Q19" s="17"/>
     </row>
-    <row r="20" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s" s="61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="39"/>
       <c r="C20" s="22"/>
@@ -2193,9 +2243,9 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s" s="61">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="39"/>
       <c r="C21" s="22"/>
@@ -2214,9 +2264,9 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="7"/>
     </row>
-    <row r="22" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s" s="56">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="46"/>
       <c r="C22" s="27"/>
@@ -2235,32 +2285,32 @@
       <c r="P22" s="11"/>
       <c r="Q22" s="16"/>
     </row>
-    <row r="23" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s" s="50">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s" s="100">
         <v>31</v>
       </c>
-      <c r="B23" t="s" s="95">
-        <v>32</v>
-      </c>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="96"/>
-      <c r="K23" s="96"/>
-      <c r="L23" s="96"/>
-      <c r="M23" s="96"/>
-      <c r="N23" s="96"/>
-      <c r="O23" s="96"/>
-      <c r="P23" s="97"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="106"/>
+      <c r="E23" s="106"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="106"/>
+      <c r="H23" s="106"/>
+      <c r="I23" s="106"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="106"/>
+      <c r="L23" s="106"/>
+      <c r="M23" s="106"/>
+      <c r="N23" s="106"/>
+      <c r="O23" s="106"/>
+      <c r="P23" s="107"/>
       <c r="Q23" s="85"/>
     </row>
-    <row r="24" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s" s="41">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="42"/>
       <c r="C24" s="30"/>
@@ -2279,9 +2329,9 @@
       <c r="P24" s="12"/>
       <c r="Q24" s="13"/>
     </row>
-    <row r="25" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s" s="61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="39"/>
       <c r="C25" s="22"/>
@@ -2300,9 +2350,9 @@
       <c r="P25" s="5"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s" s="61">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="39"/>
       <c r="C26" s="22"/>
@@ -2321,9 +2371,9 @@
       <c r="P26" s="5"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s" s="56">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" s="40"/>
       <c r="C27" s="27"/>
@@ -2342,32 +2392,32 @@
       <c r="P27" s="11"/>
       <c r="Q27" s="16"/>
     </row>
-    <row r="28" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s" s="49">
+        <v>33</v>
+      </c>
+      <c r="B28" t="s" s="116">
         <v>34</v>
       </c>
-      <c r="B28" t="s" s="100">
-        <v>35</v>
-      </c>
-      <c r="C28" s="101"/>
-      <c r="D28" s="101"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="101"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="101"/>
-      <c r="I28" s="101"/>
-      <c r="J28" s="101"/>
-      <c r="K28" s="101"/>
-      <c r="L28" s="101"/>
-      <c r="M28" s="101"/>
-      <c r="N28" s="101"/>
-      <c r="O28" s="101"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="117"/>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
+      <c r="K28" s="117"/>
+      <c r="L28" s="117"/>
+      <c r="M28" s="117"/>
+      <c r="N28" s="117"/>
+      <c r="O28" s="117"/>
       <c r="P28" s="85"/>
       <c r="Q28" s="24"/>
     </row>
-    <row r="29" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s" s="41">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" s="42"/>
       <c r="C29" s="30"/>
@@ -2386,9 +2436,9 @@
       <c r="P29" s="12"/>
       <c r="Q29" s="17"/>
     </row>
-    <row r="30" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s" s="61">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" s="39"/>
       <c r="C30" s="22"/>
@@ -2407,9 +2457,9 @@
       <c r="P30" s="5"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s" s="56">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B31" s="46"/>
       <c r="C31" s="27"/>
@@ -2428,32 +2478,32 @@
       <c r="P31" s="11"/>
       <c r="Q31" s="16"/>
     </row>
-    <row r="32" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s" s="60">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s" s="105">
         <v>36</v>
       </c>
-      <c r="B32" t="s" s="99">
+      <c r="C32" s="115"/>
+      <c r="D32" s="115"/>
+      <c r="E32" s="115"/>
+      <c r="F32" s="115"/>
+      <c r="G32" s="115"/>
+      <c r="H32" s="115"/>
+      <c r="I32" s="115"/>
+      <c r="J32" s="115"/>
+      <c r="K32" s="115"/>
+      <c r="L32" s="115"/>
+      <c r="M32" s="115"/>
+      <c r="N32" s="115"/>
+      <c r="O32" s="115"/>
+      <c r="P32" s="116"/>
+      <c r="Q32" s="24"/>
+    </row>
+    <row r="33" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s" s="63">
         <v>37</v>
-      </c>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="98"/>
-      <c r="G32" s="98"/>
-      <c r="H32" s="98"/>
-      <c r="I32" s="98"/>
-      <c r="J32" s="98"/>
-      <c r="K32" s="98"/>
-      <c r="L32" s="98"/>
-      <c r="M32" s="98"/>
-      <c r="N32" s="98"/>
-      <c r="O32" s="98"/>
-      <c r="P32" s="100"/>
-      <c r="Q32" s="24"/>
-    </row>
-    <row r="33" spans="1:17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s" s="63">
-        <v>38</v>
       </c>
       <c r="B33" s="42"/>
       <c r="C33" s="32"/>
@@ -2472,9 +2522,9 @@
       <c r="P33" s="20"/>
       <c r="Q33" s="53"/>
     </row>
-    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" t="s" s="62">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B34" s="44"/>
       <c r="C34" s="30"/>
@@ -2493,9 +2543,9 @@
       <c r="P34" s="12"/>
       <c r="Q34" s="17"/>
     </row>
-    <row r="35" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s" s="52">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B35" s="45"/>
       <c r="C35" s="33"/>
@@ -2514,32 +2564,32 @@
       <c r="P35" s="20"/>
       <c r="Q35" s="21"/>
     </row>
-    <row r="36" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s" s="49">
+        <v>38</v>
+      </c>
+      <c r="B36" t="s" s="100">
         <v>39</v>
       </c>
-      <c r="B36" t="s" s="95">
+      <c r="C36" s="115"/>
+      <c r="D36" s="115"/>
+      <c r="E36" s="115"/>
+      <c r="F36" s="115"/>
+      <c r="G36" s="115"/>
+      <c r="H36" s="115"/>
+      <c r="I36" s="115"/>
+      <c r="J36" s="115"/>
+      <c r="K36" s="115"/>
+      <c r="L36" s="115"/>
+      <c r="M36" s="115"/>
+      <c r="N36" s="115"/>
+      <c r="O36" s="115"/>
+      <c r="P36" s="107"/>
+      <c r="Q36" s="24"/>
+    </row>
+    <row r="37" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s" s="64">
         <v>40</v>
-      </c>
-      <c r="C36" s="98"/>
-      <c r="D36" s="98"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="98"/>
-      <c r="H36" s="98"/>
-      <c r="I36" s="98"/>
-      <c r="J36" s="98"/>
-      <c r="K36" s="98"/>
-      <c r="L36" s="98"/>
-      <c r="M36" s="98"/>
-      <c r="N36" s="98"/>
-      <c r="O36" s="98"/>
-      <c r="P36" s="97"/>
-      <c r="Q36" s="24"/>
-    </row>
-    <row r="37" spans="1:17" ht="17.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s" s="64">
-        <v>41</v>
       </c>
       <c r="B37" s="65"/>
       <c r="C37" s="66"/>
@@ -2560,31 +2610,39 @@
         <f>SUM(B37,C37,D37,E37,F37,G37,H37,I37,J37,K37,L37,M37,N37,O37)</f>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s" s="88">
+    <row r="38" spans="1:17" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s" s="108">
+        <v>41</v>
+      </c>
+      <c r="B38" s="109"/>
+      <c r="C38" s="109"/>
+      <c r="D38" s="109"/>
+      <c r="E38" s="110"/>
+      <c r="F38" s="110"/>
+      <c r="G38" s="111"/>
+      <c r="H38" t="s" s="108">
         <v>42</v>
       </c>
-      <c r="B38" s="89"/>
-      <c r="C38" s="89"/>
-      <c r="D38" s="89"/>
-      <c r="E38" s="90"/>
-      <c r="F38" s="90"/>
-      <c r="G38" s="91"/>
-      <c r="H38" t="s" s="88">
-        <v>43</v>
-      </c>
-      <c r="I38" s="90"/>
-      <c r="J38" s="90"/>
-      <c r="K38" s="90"/>
-      <c r="L38" s="90"/>
-      <c r="M38" s="90"/>
-      <c r="N38" s="90"/>
-      <c r="O38" s="90"/>
-      <c r="P38" s="90"/>
-      <c r="Q38" s="91"/>
+      <c r="I38" s="110"/>
+      <c r="J38" s="110"/>
+      <c r="K38" s="110"/>
+      <c r="L38" s="110"/>
+      <c r="M38" s="110"/>
+      <c r="N38" s="110"/>
+      <c r="O38" s="110"/>
+      <c r="P38" s="110"/>
+      <c r="Q38" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A38:G38"/>
+    <mergeCell ref="H38:Q38"/>
+    <mergeCell ref="A17:Q17"/>
+    <mergeCell ref="B18:P18"/>
+    <mergeCell ref="B23:P23"/>
+    <mergeCell ref="B36:P36"/>
+    <mergeCell ref="B32:P32"/>
+    <mergeCell ref="B28:O28"/>
     <mergeCell ref="B11:P11"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="I2:L2"/>
@@ -2593,14 +2651,6 @@
     <mergeCell ref="B9:O9"/>
     <mergeCell ref="O2:Q2"/>
     <mergeCell ref="B5:P5"/>
-    <mergeCell ref="A38:G38"/>
-    <mergeCell ref="H38:Q38"/>
-    <mergeCell ref="A17:Q17"/>
-    <mergeCell ref="B18:P18"/>
-    <mergeCell ref="B23:P23"/>
-    <mergeCell ref="B36:P36"/>
-    <mergeCell ref="B32:P32"/>
-    <mergeCell ref="B28:O28"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2621,14 +2671,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s" s="9">
+        <v>43</v>
+      </c>
+      <c r="B1" t="s" s="122">
         <v>44</v>
-      </c>
-      <c r="B1" t="s" s="122">
-        <v>45</v>
       </c>
       <c r="C1" s="123"/>
       <c r="D1" s="123"/>
@@ -2637,11 +2687,11 @@
       <c r="G1" s="123"/>
       <c r="H1" s="124"/>
       <c r="I1" t="s" s="125">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J1" s="126"/>
     </row>
-    <row r="2" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="74"/>
       <c r="B2" s="121"/>
       <c r="C2" s="120"/>
@@ -2653,7 +2703,7 @@
       <c r="I2" s="118"/>
       <c r="J2" s="119"/>
     </row>
-    <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="74"/>
       <c r="B3" s="75"/>
       <c r="C3" s="76"/>
@@ -2665,7 +2715,7 @@
       <c r="I3" s="86"/>
       <c r="J3" s="87"/>
     </row>
-    <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="74"/>
       <c r="B4" s="121"/>
       <c r="C4" s="120"/>
@@ -2677,7 +2727,7 @@
       <c r="I4" s="118"/>
       <c r="J4" s="119"/>
     </row>
-    <row r="5" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="74"/>
       <c r="B5" s="121"/>
       <c r="C5" s="120"/>
@@ -2689,7 +2739,7 @@
       <c r="I5" s="118"/>
       <c r="J5" s="119"/>
     </row>
-    <row r="6" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="74"/>
       <c r="B6" s="121"/>
       <c r="C6" s="120"/>
@@ -2701,7 +2751,7 @@
       <c r="I6" s="118"/>
       <c r="J6" s="119"/>
     </row>
-    <row r="7" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="121"/>
       <c r="C7" s="120"/>
@@ -2713,7 +2763,7 @@
       <c r="I7" s="118"/>
       <c r="J7" s="119"/>
     </row>
-    <row r="8" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18"/>
       <c r="B8" s="121"/>
       <c r="C8" s="120"/>
@@ -2725,7 +2775,7 @@
       <c r="I8" s="118"/>
       <c r="J8" s="119"/>
     </row>
-    <row r="9" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="121"/>
       <c r="C9" s="120"/>
@@ -2737,7 +2787,7 @@
       <c r="I9" s="118"/>
       <c r="J9" s="119"/>
     </row>
-    <row r="10" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="118"/>
       <c r="C10" s="120"/>
@@ -2749,7 +2799,7 @@
       <c r="I10" s="118"/>
       <c r="J10" s="119"/>
     </row>
-    <row r="11" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="118"/>
       <c r="C11" s="120"/>
@@ -2761,7 +2811,7 @@
       <c r="I11" s="118"/>
       <c r="J11" s="119"/>
     </row>
-    <row r="12" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="118"/>
       <c r="C12" s="120"/>
@@ -2773,7 +2823,7 @@
       <c r="I12" s="118"/>
       <c r="J12" s="119"/>
     </row>
-    <row r="13" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="118"/>
       <c r="C13" s="120"/>
@@ -2785,7 +2835,7 @@
       <c r="I13" s="118"/>
       <c r="J13" s="119"/>
     </row>
-    <row r="14" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="118"/>
       <c r="C14" s="120"/>
@@ -2797,7 +2847,7 @@
       <c r="I14" s="118"/>
       <c r="J14" s="119"/>
     </row>
-    <row r="15" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="118"/>
       <c r="C15" s="120"/>
@@ -2809,7 +2859,7 @@
       <c r="I15" s="118"/>
       <c r="J15" s="119"/>
     </row>
-    <row r="16" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="118"/>
       <c r="C16" s="120"/>
@@ -2821,7 +2871,7 @@
       <c r="I16" s="118"/>
       <c r="J16" s="119"/>
     </row>
-    <row r="17" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="118"/>
       <c r="C17" s="120"/>
@@ -2833,7 +2883,7 @@
       <c r="I17" s="118"/>
       <c r="J17" s="119"/>
     </row>
-    <row r="18" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="118"/>
       <c r="C18" s="120"/>
@@ -2845,7 +2895,7 @@
       <c r="I18" s="118"/>
       <c r="J18" s="119"/>
     </row>
-    <row r="19" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="118"/>
       <c r="C19" s="120"/>
@@ -2857,7 +2907,7 @@
       <c r="I19" s="118"/>
       <c r="J19" s="119"/>
     </row>
-    <row r="20" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="118"/>
       <c r="C20" s="120"/>
@@ -2869,7 +2919,7 @@
       <c r="I20" s="118"/>
       <c r="J20" s="119"/>
     </row>
-    <row r="21" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="118"/>
       <c r="C21" s="120"/>
@@ -2881,10 +2931,10 @@
       <c r="I21" s="118"/>
       <c r="J21" s="119"/>
     </row>
-    <row r="22" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" t="s" s="121">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="120"/>
       <c r="D22" s="120"/>
@@ -2895,7 +2945,7 @@
       <c r="I22" s="118"/>
       <c r="J22" s="119"/>
     </row>
-    <row r="23" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="18"/>
       <c r="B23" s="118"/>
       <c r="C23" s="120"/>
@@ -2907,7 +2957,7 @@
       <c r="I23" s="118"/>
       <c r="J23" s="119"/>
     </row>
-    <row r="24" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="118"/>
       <c r="C24" s="120"/>
@@ -2919,7 +2969,7 @@
       <c r="I24" s="118"/>
       <c r="J24" s="119"/>
     </row>
-    <row r="25" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="118"/>
       <c r="C25" s="120"/>
@@ -2931,7 +2981,7 @@
       <c r="I25" s="118"/>
       <c r="J25" s="119"/>
     </row>
-    <row r="26" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="118"/>
       <c r="C26" s="120"/>
@@ -2943,7 +2993,7 @@
       <c r="I26" s="118"/>
       <c r="J26" s="119"/>
     </row>
-    <row r="27" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="118"/>
       <c r="C27" s="120"/>
@@ -2955,7 +3005,7 @@
       <c r="I27" s="118"/>
       <c r="J27" s="119"/>
     </row>
-    <row r="28" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18"/>
       <c r="B28" s="118"/>
       <c r="C28" s="120"/>
@@ -2967,7 +3017,7 @@
       <c r="I28" s="118"/>
       <c r="J28" s="119"/>
     </row>
-    <row r="29" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="118"/>
       <c r="C29" s="120"/>
@@ -2979,7 +3029,7 @@
       <c r="I29" s="118"/>
       <c r="J29" s="119"/>
     </row>
-    <row r="30" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="118"/>
       <c r="C30" s="120"/>
@@ -2991,7 +3041,7 @@
       <c r="I30" s="118"/>
       <c r="J30" s="119"/>
     </row>
-    <row r="31" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="118"/>
       <c r="C31" s="120"/>
@@ -3003,7 +3053,7 @@
       <c r="I31" s="118"/>
       <c r="J31" s="119"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="10"/>
       <c r="B32" s="10"/>
       <c r="C32" s="10"/>
@@ -3015,7 +3065,7 @@
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="10"/>
       <c r="C33" s="10"/>
@@ -3027,7 +3077,7 @@
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="10"/>
       <c r="B34" s="10"/>
       <c r="C34" s="10"/>
@@ -3039,7 +3089,7 @@
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="10"/>
       <c r="B35" s="10"/>
       <c r="C35" s="10"/>
@@ -3051,7 +3101,7 @@
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="10"/>
       <c r="C36" s="10"/>
@@ -3063,7 +3113,7 @@
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="10"/>
       <c r="B37" s="10"/>
       <c r="C37" s="10"/>
@@ -3077,35 +3127,28 @@
     </row>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="B12:H12"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B18:H18"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="B15:H15"/>
-    <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="B27:H27"/>
-    <mergeCell ref="B20:H20"/>
-    <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B23:H23"/>
-    <mergeCell ref="B26:H26"/>
-    <mergeCell ref="B24:H24"/>
-    <mergeCell ref="B25:H25"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B30:H30"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="I10:J10"/>
@@ -3115,28 +3158,35 @@
     <mergeCell ref="B7:H7"/>
     <mergeCell ref="B8:H8"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="B29:H29"/>
-    <mergeCell ref="B30:H30"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="I24:J24"/>
-    <mergeCell ref="I25:J25"/>
-    <mergeCell ref="I26:J26"/>
-    <mergeCell ref="I27:J27"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="B27:H27"/>
+    <mergeCell ref="B20:H20"/>
+    <mergeCell ref="B21:H21"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="B26:H26"/>
+    <mergeCell ref="B24:H24"/>
+    <mergeCell ref="B25:H25"/>
+    <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="B15:H15"/>
+    <mergeCell ref="B16:H16"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B13:H13"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>